<commit_message>
Add drop down menu (not fully functional).
</commit_message>
<xml_diff>
--- a/Master-Location.xlsx
+++ b/Master-Location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ece0b9607a390b55/Documents/UAlberta 2023-2024 Year 4/Winter 2024/FIN 488 FINTECH3/ABpower_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1FD4F38D-BAC4-4687-AC97-992191EF3289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E615FF-356F-4BF4-880C-6864F755349C}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{1FD4F38D-BAC4-4687-AC97-992191EF3289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA5E7057-CC14-470E-8F52-1EE1B3B0CCCF}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="705" windowWidth="15120" windowHeight="9713" tabRatio="703" xr2:uid="{806FED5A-1E2A-4469-B161-9D1FCB3CC681}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="664">
   <si>
     <t>Document:</t>
   </si>
@@ -2033,9 +2033,6 @@
   </si>
   <si>
     <t>Public — August 16, 2022</t>
-  </si>
-  <si>
-    <t>ASSET</t>
   </si>
 </sst>
 </file>
@@ -2162,10 +2159,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2467,7 +2460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078BE2D0-CC28-442D-81D1-66D4DB4F45E2}">
   <dimension ref="A1:L264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2542,7 +2535,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>664</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>

</xml_diff>